<commit_message>
filled in full sheet
</commit_message>
<xml_diff>
--- a/Design Input Files/Design Input File_Student_Blank_V25-00.xlsx
+++ b/Design Input Files/Design Input File_Student_Blank_V25-00.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasnussbaumer/Documents/MATLAB/ASEN 2804/ASEN-2804-Lab/Aero and Weight/Design Input Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\katya\Desktop\ASEN 2804\ASEN2804_AeroModeling\Design Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBBAC6B-33E1-2448-A6E1-C2214DB386F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45875499-0A8F-4CC5-9CEF-D6153DC88D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{904FC4B5-3CDE-421B-8E98-23A2C72E8C1E}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" activeTab="1" xr2:uid="{904FC4B5-3CDE-421B-8E98-23A2C72E8C1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Variable Reference" sheetId="8" r:id="rId1"/>
@@ -3380,16 +3380,16 @@
       <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="104.5" style="5" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="104.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>192</v>
       </c>
@@ -3403,7 +3403,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>246</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>246</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>246</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>246</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>246</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>246</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>246</v>
       </c>
@@ -3502,7 +3502,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>246</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>246</v>
       </c>
@@ -3530,7 +3530,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>246</v>
       </c>
@@ -3544,7 +3544,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>246</v>
       </c>
@@ -3558,7 +3558,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>246</v>
       </c>
@@ -3572,7 +3572,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>246</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>246</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>246</v>
       </c>
@@ -3614,7 +3614,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>246</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>246</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>246</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>246</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>246</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>246</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>246</v>
       </c>
@@ -3712,7 +3712,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>246</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>246</v>
       </c>
@@ -3740,7 +3740,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>246</v>
       </c>
@@ -3754,7 +3754,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>246</v>
       </c>
@@ -3768,7 +3768,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>246</v>
       </c>
@@ -3782,7 +3782,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>246</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>246</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>246</v>
       </c>
@@ -3824,7 +3824,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>246</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>246</v>
       </c>
@@ -3852,7 +3852,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>246</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>246</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>246</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>246</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>246</v>
       </c>
@@ -3922,7 +3922,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>246</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>246</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>246</v>
       </c>
@@ -3964,7 +3964,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>246</v>
       </c>
@@ -3978,7 +3978,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>246</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>246</v>
       </c>
@@ -4006,7 +4006,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
         <v>246</v>
       </c>
@@ -4020,7 +4020,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>246</v>
       </c>
@@ -4034,7 +4034,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
         <v>246</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>246</v>
       </c>
@@ -4062,7 +4062,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>246</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>246</v>
       </c>
@@ -4090,7 +4090,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
         <v>246</v>
       </c>
@@ -4104,7 +4104,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>246</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>246</v>
       </c>
@@ -4132,7 +4132,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>246</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>246</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>246</v>
       </c>
@@ -4174,7 +4174,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>246</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>246</v>
       </c>
@@ -4202,7 +4202,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>246</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>193</v>
       </c>
@@ -4230,7 +4230,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>193</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>193</v>
       </c>
@@ -4258,7 +4258,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>193</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>193</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>193</v>
       </c>
@@ -4300,7 +4300,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>193</v>
       </c>
@@ -4314,7 +4314,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>193</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>193</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>193</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>193</v>
       </c>
@@ -4370,7 +4370,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>193</v>
       </c>
@@ -4384,7 +4384,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>193</v>
       </c>
@@ -4398,7 +4398,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>193</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>193</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>193</v>
       </c>
@@ -4440,7 +4440,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>193</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>193</v>
       </c>
@@ -4468,7 +4468,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>235</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>235</v>
       </c>
@@ -4497,7 +4497,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>235</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>235</v>
       </c>
@@ -4525,7 +4525,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>235</v>
       </c>
@@ -4539,7 +4539,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>235</v>
       </c>
@@ -4553,7 +4553,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>235</v>
       </c>
@@ -4567,7 +4567,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>235</v>
       </c>
@@ -4581,7 +4581,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>235</v>
       </c>
@@ -4595,7 +4595,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>235</v>
       </c>
@@ -4609,7 +4609,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>235</v>
       </c>
@@ -4623,7 +4623,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
         <v>235</v>
       </c>
@@ -4637,7 +4637,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>235</v>
       </c>
@@ -4651,7 +4651,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>235</v>
       </c>
@@ -4665,7 +4665,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>235</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
         <v>235</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
         <v>235</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
         <v>235</v>
       </c>
@@ -4721,7 +4721,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>235</v>
       </c>
@@ -4735,7 +4735,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="97" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
         <v>235</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>235</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
         <v>235</v>
       </c>
@@ -4777,7 +4777,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>235</v>
       </c>
@@ -4791,7 +4791,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>235</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>235</v>
       </c>
@@ -4819,7 +4819,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="6" t="s">
         <v>235</v>
       </c>
@@ -4843,37 +4843,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28ADD393-55AB-49FB-9382-D2896E9EB980}">
   <dimension ref="A1:BF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="BF3" sqref="BF3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="7"/>
-    <col min="2" max="2" width="10.5" style="7" customWidth="1"/>
-    <col min="3" max="11" width="8.83203125" style="7"/>
-    <col min="12" max="12" width="15.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.83203125" style="7" customWidth="1"/>
-    <col min="14" max="14" width="8.83203125" style="7"/>
+    <col min="1" max="1" width="8.85546875" style="7"/>
+    <col min="2" max="2" width="10.42578125" style="7" customWidth="1"/>
+    <col min="3" max="11" width="8.85546875" style="7"/>
+    <col min="12" max="12" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" style="7" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="7"/>
     <col min="15" max="15" width="12" style="7" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="8.83203125" style="7"/>
-    <col min="18" max="18" width="16.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.83203125" style="7"/>
-    <col min="20" max="20" width="15.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="21" max="27" width="8.83203125" style="7"/>
-    <col min="28" max="28" width="15.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="29" max="38" width="8.83203125" style="7"/>
+    <col min="16" max="17" width="8.85546875" style="7"/>
+    <col min="18" max="18" width="16.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" style="7"/>
+    <col min="20" max="20" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="27" width="8.85546875" style="7"/>
+    <col min="28" max="28" width="15.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="29" max="38" width="8.85546875" style="7"/>
     <col min="39" max="39" width="12" style="7" bestFit="1" customWidth="1"/>
-    <col min="40" max="43" width="8.83203125" style="7"/>
-    <col min="44" max="44" width="16.6640625" style="7" customWidth="1"/>
-    <col min="45" max="52" width="8.83203125" style="7"/>
-    <col min="53" max="54" width="9.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="9.1640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="9.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="57" max="16384" width="8.83203125" style="7"/>
+    <col min="40" max="43" width="8.85546875" style="7"/>
+    <col min="44" max="44" width="16.7109375" style="7" customWidth="1"/>
+    <col min="45" max="52" width="8.85546875" style="7"/>
+    <col min="53" max="54" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="9.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="57" max="16384" width="8.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>45</v>
       </c>
@@ -5049,7 +5049,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:58" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:58" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>266</v>
       </c>
@@ -5206,14 +5206,26 @@
       <c r="AZ2" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="BA2" s="33"/>
-      <c r="BB2" s="33"/>
-      <c r="BC2" s="33"/>
-      <c r="BD2" s="33"/>
-      <c r="BE2" s="33"/>
-      <c r="BF2" s="33"/>
-    </row>
-    <row r="21" s="29" customFormat="1" x14ac:dyDescent="0.2"/>
+      <c r="BA2" s="33">
+        <v>2</v>
+      </c>
+      <c r="BB2" s="33">
+        <v>500</v>
+      </c>
+      <c r="BC2" s="33">
+        <v>40</v>
+      </c>
+      <c r="BD2" s="33">
+        <v>0</v>
+      </c>
+      <c r="BE2" s="33">
+        <v>270</v>
+      </c>
+      <c r="BF2" s="33">
+        <v>2.23</v>
+      </c>
+    </row>
+    <row r="21" s="29" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T51 AR2:AR51 AZ2:AZ51 AJ2:AJ51 AB2:AB51 L2 L4:L51" xr:uid="{F18DD44F-5AC9-42F9-970E-83AFBD39DB9D}">
@@ -5233,25 +5245,25 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="18"/>
-    <col min="2" max="2" width="11.83203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="42" width="8.83203125" style="18"/>
-    <col min="43" max="43" width="11.83203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="8.83203125" style="18"/>
-    <col min="45" max="45" width="9.83203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.83203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.83203125" style="18"/>
-    <col min="48" max="48" width="10.33203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.1640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="8.83203125" style="18"/>
-    <col min="51" max="51" width="10.1640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="11.83203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="53" max="16384" width="8.83203125" style="18"/>
+    <col min="1" max="1" width="8.85546875" style="18"/>
+    <col min="2" max="2" width="11.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="42" width="8.85546875" style="18"/>
+    <col min="43" max="43" width="11.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="8.85546875" style="18"/>
+    <col min="45" max="45" width="9.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.85546875" style="18"/>
+    <col min="48" max="48" width="10.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="8.85546875" style="18"/>
+    <col min="51" max="51" width="10.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="53" max="16384" width="8.85546875" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>45</v>
       </c>
@@ -5415,7 +5427,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:54" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:54" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="str">
         <f>Main_Input!A2</f>
         <v>Tempest</v>
@@ -5580,7 +5592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="X3" s="19"/>
       <c r="Y3" s="19"/>
       <c r="Z3" s="19"/>
@@ -5600,7 +5612,7 @@
       <c r="AN3" s="19"/>
       <c r="AO3" s="19"/>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="X4" s="19"/>
       <c r="Y4" s="19"/>
       <c r="Z4" s="19"/>
@@ -5620,7 +5632,7 @@
       <c r="AN4" s="19"/>
       <c r="AO4" s="19"/>
     </row>
-    <row r="21" s="30" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" s="30" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5635,20 +5647,20 @@
       <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="8.83203125" style="1"/>
+    <col min="1" max="6" width="8.85546875" style="1"/>
     <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="21" width="8.83203125" style="1"/>
-    <col min="22" max="22" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.1640625" style="1" customWidth="1"/>
-    <col min="24" max="25" width="8.83203125" style="1"/>
-    <col min="26" max="26" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="8.83203125" style="1"/>
+    <col min="8" max="21" width="8.85546875" style="1"/>
+    <col min="22" max="22" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.140625" style="1" customWidth="1"/>
+    <col min="24" max="25" width="8.85546875" style="1"/>
+    <col min="26" max="26" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>45</v>
       </c>
@@ -5731,7 +5743,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="str">
         <f>Main_Input!A2</f>
         <v>Tempest</v>
@@ -5815,7 +5827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -5844,7 +5856,7 @@
       <c r="Z3" s="7"/>
       <c r="AA3" s="7"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -5873,7 +5885,7 @@
       <c r="Z4" s="7"/>
       <c r="AA4" s="7"/>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -5902,7 +5914,7 @@
       <c r="Z5" s="7"/>
       <c r="AA5" s="7"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -5931,7 +5943,7 @@
       <c r="Z6" s="7"/>
       <c r="AA6" s="7"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -5960,7 +5972,7 @@
       <c r="Z7" s="7"/>
       <c r="AA7" s="7"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -5989,7 +6001,7 @@
       <c r="Z8" s="7"/>
       <c r="AA8" s="7"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -6018,7 +6030,7 @@
       <c r="Z9" s="7"/>
       <c r="AA9" s="7"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -6047,7 +6059,7 @@
       <c r="Z10" s="7"/>
       <c r="AA10" s="7"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -6076,7 +6088,7 @@
       <c r="Z11" s="7"/>
       <c r="AA11" s="7"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -6105,7 +6117,7 @@
       <c r="Z12" s="7"/>
       <c r="AA12" s="7"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -6134,7 +6146,7 @@
       <c r="Z13" s="7"/>
       <c r="AA13" s="7"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -6163,7 +6175,7 @@
       <c r="Z14" s="7"/>
       <c r="AA14" s="7"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -6192,7 +6204,7 @@
       <c r="Z15" s="7"/>
       <c r="AA15" s="7"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -6221,7 +6233,7 @@
       <c r="Z16" s="7"/>
       <c r="AA16" s="7"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -6250,7 +6262,7 @@
       <c r="Z17" s="7"/>
       <c r="AA17" s="7"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -6279,7 +6291,7 @@
       <c r="Z18" s="7"/>
       <c r="AA18" s="7"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -6308,7 +6320,7 @@
       <c r="Z19" s="7"/>
       <c r="AA19" s="7"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -6337,7 +6349,7 @@
       <c r="Z20" s="7"/>
       <c r="AA20" s="7"/>
     </row>
-    <row r="21" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6353,18 +6365,18 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" customWidth="1"/>
-    <col min="7" max="8" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="8" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>102</v>
       </c>
@@ -6390,7 +6402,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>20.8</v>
       </c>
@@ -6416,7 +6428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>106</v>
       </c>
@@ -6457,9 +6469,9 @@
       <selection activeCell="V27" sqref="V27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>99</v>
       </c>
@@ -6470,7 +6482,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>-5</v>
       </c>
@@ -6481,7 +6493,7 @@
         <v>4.4250999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>-4</v>
       </c>
@@ -6492,7 +6504,7 @@
         <v>3.3783000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>-3</v>
       </c>
@@ -6503,7 +6515,7 @@
         <v>2.8627E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>-2</v>
       </c>
@@ -6514,7 +6526,7 @@
         <v>2.5864000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>-1</v>
       </c>
@@ -6525,7 +6537,7 @@
         <v>2.4643000000000002E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>0</v>
       </c>
@@ -6536,7 +6548,7 @@
         <v>2.5099E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -6547,7 +6559,7 @@
         <v>2.5635000000000002E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>2</v>
       </c>
@@ -6558,7 +6570,7 @@
         <v>2.7660000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>3</v>
       </c>
@@ -6569,7 +6581,7 @@
         <v>3.0676999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>4</v>
       </c>
@@ -6580,7 +6592,7 @@
         <v>3.4854999999999997E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>5</v>
       </c>
@@ -6591,7 +6603,7 @@
         <v>4.0403000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>6</v>
       </c>
@@ -6602,7 +6614,7 @@
         <v>4.759E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>7</v>
       </c>
@@ -6613,7 +6625,7 @@
         <v>5.7107999999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>8</v>
       </c>
@@ -6624,7 +6636,7 @@
         <v>7.0132E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>9</v>
       </c>
@@ -6635,7 +6647,7 @@
         <v>9.0921000000000002E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>10</v>
       </c>
@@ -6646,7 +6658,7 @@
         <v>0.11193</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>11</v>
       </c>
@@ -6657,7 +6669,7 @@
         <v>0.13253999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>12</v>
       </c>
@@ -6668,7 +6680,7 @@
         <v>0.15645000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E21" s="4"/>
       <c r="F21" s="14"/>
     </row>
@@ -6686,7 +6698,7 @@
       <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>